<commit_message>
Los years en planilla Data se deben rellenar a mano
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felipe.garcia\Codigos\Codigo_AF_FG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E22696-3480-4AA7-B591-AC467C42916B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4995CD9C-9146-40BF-BD63-37A54D4FC424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{35335E33-6303-42E7-B1FE-4926957C372B}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
desarrollo funciones Fit_distribs y probs
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felipe.garcia\Codigos\Codigo_AF_FG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4995CD9C-9146-40BF-BD63-37A54D4FC424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE1AACA-9406-4247-9239-F091952B1989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{35335E33-6303-42E7-B1FE-4926957C372B}"/>
+    <workbookView xWindow="-17310" yWindow="1110" windowWidth="13410" windowHeight="14325" xr2:uid="{35335E33-6303-42E7-B1FE-4926957C372B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>ID</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Calama</t>
+  </si>
+  <si>
+    <t>Calama 2</t>
   </si>
 </sst>
 </file>
@@ -98,11 +101,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{211948CE-5B54-47DE-A733-A13983CDDD41}">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -428,7 +434,7 @@
     <col min="2" max="23" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,471 +442,634 @@
         <f t="shared" ref="B1" si="0">+B4</f>
         <v>Calama</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="2">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" s="4">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" s="2">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" s="4">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" s="2">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" s="4">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" s="2">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="B12" s="2">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" s="4">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>11</v>
       </c>
       <c r="B15" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>13</v>
       </c>
       <c r="B17" s="2">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>14</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>15</v>
       </c>
       <c r="B19" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>17</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>18</v>
       </c>
       <c r="B22" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>19</v>
       </c>
       <c r="B23">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" s="4">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>20</v>
       </c>
       <c r="B24">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" s="4">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>21</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>22</v>
       </c>
       <c r="B26">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>23</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>24</v>
       </c>
       <c r="B28">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" s="4">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>25</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>26</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>27</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>28</v>
       </c>
       <c r="B32">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32" s="4">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>29</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>30</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>31</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>32</v>
       </c>
       <c r="B36">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36" s="4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>33</v>
       </c>
       <c r="B37">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>34</v>
       </c>
       <c r="B38">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>35</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>36</v>
       </c>
       <c r="B40">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>37</v>
       </c>
       <c r="B41">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41" s="4">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>38</v>
       </c>
       <c r="B42">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42" s="4">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>39</v>
       </c>
       <c r="B43">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43" s="4">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>40</v>
       </c>
       <c r="B44">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>41</v>
       </c>
       <c r="B45">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C45" s="4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>42</v>
       </c>
       <c r="B46">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>43</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>44</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>45</v>
       </c>
       <c r="B49">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>46</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C50" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>47</v>
       </c>
       <c r="B51">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C51" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>48</v>
       </c>
       <c r="B52">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>49</v>
       </c>
       <c r="B53">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C53" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>50</v>
       </c>
       <c r="B54">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C54" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>51</v>
       </c>
       <c r="B55">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C55" s="4">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>52</v>
       </c>
       <c r="B56">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C56" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>53</v>
       </c>
       <c r="B57">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C57" s="4">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>54</v>
       </c>
       <c r="B58">
+        <v>3.5</v>
+      </c>
+      <c r="C58" s="4">
         <v>3.5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008BE237BB54F80145B3517CAF33BD3493" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d860eedc6b51c00ad9fdd9b4c7ddf6e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="407453d4-625b-4198-9db6-120c6918a4e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="15d62e9d9f570863c95abd63cc9aaf72" ns2:_="">
     <xsd:import namespace="407453d4-625b-4198-9db6-120c6918a4e9"/>
@@ -1038,21 +1207,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9D6FFFD-90CD-4DB6-B39E-1AC6DEFD38C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D489442B-AB6B-41DC-A521-F1205F978AB2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1070,7 +1240,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E701F88B-2FF2-49E8-8D57-722A52B01DFD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1081,4 +1251,12 @@
     <ds:schemaRef ds:uri="586d46c3-db18-4005-abe1-ae1f8efa73aa"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9D6FFFD-90CD-4DB6-B39E-1AC6DEFD38C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>